<commit_message>
Finalizováno: Bombátor načítá CSV
Bombátor nyní správně načítá CSV soubory místo excel souborů
Nicméně způsob jak jsou konvertovány id učitelů ze str na list[int] je minimálně pochybný z hlediska efektivity, takže někdo by se na to asi mohl kouknout yk
</commit_message>
<xml_diff>
--- a/results/bez_garanta.xlsx
+++ b/results/bez_garanta.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
   <si>
     <t>zkratka</t>
   </si>
@@ -195,8 +195,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:F26" totalsRowShown="0">
-  <autoFilter ref="A1:F26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Frame0" displayName="Frame0" ref="A1:F18" totalsRowShown="0">
+  <autoFilter ref="A1:F18"/>
   <tableColumns count="6">
     <tableColumn id="1" name="zkratka" dataDxfId="0"/>
     <tableColumn id="2" name="rok" dataDxfId="1"/>
@@ -494,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -602,323 +602,195 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2">
         <v>2023</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>2023</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>2023</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2">
         <v>2023</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2">
         <v>2023</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2">
         <v>2023</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2">
         <v>2023</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
         <v>2023</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2">
         <v>2023</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2">
         <v>2023</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2">
         <v>2023</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2">
         <v>2023</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pohled fakulty: Strict mode bypass
Bypass strict mode při castování str -> i64 skrze nahrazení stringů s délkou 0 hodnotou null.

Jen zběžná kontrola dat, nutno zkontrolovat v celku.
</commit_message>
<xml_diff>
--- a/results/bez_garanta.xlsx
+++ b/results/bez_garanta.xlsx
@@ -451,12 +451,12 @@
     <t>PVK - Mikroprocesorová technika</t>
   </si>
   <si>
+    <t>PVK - Automatizované měřící systémy</t>
+  </si>
+  <si>
     <t>Biochemická cvičení</t>
   </si>
   <si>
-    <t>PVK - Automatizované měřící systémy</t>
-  </si>
-  <si>
     <t>Diplomová práce z chemie</t>
   </si>
   <si>
@@ -526,12 +526,12 @@
     <t>Anglický jazyk pro doktorandy</t>
   </si>
   <si>
+    <t>SZZ - matematika s didaktikou</t>
+  </si>
+  <si>
     <t>SZZ - Geografie s didaktikou</t>
   </si>
   <si>
-    <t>SZZ - matematika s didaktikou</t>
-  </si>
-  <si>
     <t>SZZ - biologie s didaktikou</t>
   </si>
   <si>
@@ -547,81 +547,81 @@
     <t>Aplikovaná geografie - Cestovní ruch</t>
   </si>
   <si>
+    <t>Nanotechnologie</t>
+  </si>
+  <si>
+    <t>Aplikovaná geografie - Krajina a GIS</t>
+  </si>
+  <si>
     <t>Informační technologie</t>
   </si>
   <si>
-    <t>Nanotechnologie</t>
-  </si>
-  <si>
-    <t>Aplikovaná geografie - Krajina a GIS</t>
-  </si>
-  <si>
     <t>Matematika s aplikacemi</t>
   </si>
   <si>
+    <t>SZZ - Evropská integrace a EU</t>
+  </si>
+  <si>
     <t>SZZ - Chemie</t>
   </si>
   <si>
     <t>Počítačové modelování</t>
   </si>
   <si>
-    <t>SZZ - Evropská integrace a EU</t>
-  </si>
-  <si>
     <t>Statistika a zpracování dat</t>
   </si>
   <si>
+    <t>Chemie a didaktika chemie pro SŠ</t>
+  </si>
+  <si>
+    <t>Geografie krajiny a GIS</t>
+  </si>
+  <si>
     <t>Biologie s didaktikou pro SŠ</t>
   </si>
   <si>
     <t>SZZ - Fyzika s didaktikou pro SŠ</t>
   </si>
   <si>
-    <t>Geografie krajiny a GIS</t>
-  </si>
-  <si>
-    <t>Chemie a didaktika chemie pro SŠ</t>
-  </si>
-  <si>
     <t>Geografie venkova a sídel</t>
   </si>
   <si>
     <t>Regionální geografie a cestovní ruch</t>
   </si>
   <si>
+    <t>SZZ - Toxikologie a analýza škodlivin</t>
+  </si>
+  <si>
+    <t>SZZ - numerická matematika</t>
+  </si>
+  <si>
     <t>SZZ - Reg. geografie a reg. rozvoj Česka</t>
   </si>
   <si>
-    <t>SZZ - Toxikologie a analýza škodlivin</t>
-  </si>
-  <si>
-    <t>SZZ - numerická matematika</t>
+    <t>Biologie pro vzdělávání</t>
   </si>
   <si>
     <t>Geografie pro vzdělávání</t>
   </si>
   <si>
-    <t>Biologie pro vzdělávání</t>
+    <t>Fyzika pro vzdělávání</t>
   </si>
   <si>
     <t>Matematika pro vzdělávání</t>
   </si>
   <si>
-    <t>Fyzika pro vzdělávání</t>
-  </si>
-  <si>
     <t>Chemie pro vzdělávání</t>
   </si>
   <si>
     <t>Analytická chemie</t>
   </si>
   <si>
+    <t>Fyzika</t>
+  </si>
+  <si>
     <t>SZZ - Biologie</t>
   </si>
   <si>
-    <t>Fyzika</t>
-  </si>
-  <si>
     <t>SZZ- Regionální geografie Evropy a světa</t>
   </si>
   <si>
@@ -640,24 +640,24 @@
     <t>Matematika</t>
   </si>
   <si>
+    <t>SZZ - Informatika</t>
+  </si>
+  <si>
+    <t>Chemie</t>
+  </si>
+  <si>
     <t>SZZ - Geografie</t>
   </si>
   <si>
-    <t>Chemie</t>
-  </si>
-  <si>
-    <t>SZZ - Informatika</t>
+    <t>SZZ - Obecná geografie</t>
+  </si>
+  <si>
+    <t>Matematická informatika</t>
   </si>
   <si>
     <t>Elektronika a elektrotechnika</t>
   </si>
   <si>
-    <t>Matematická informatika</t>
-  </si>
-  <si>
-    <t>SZZ - Obecná geografie</t>
-  </si>
-  <si>
     <t>SZZ - Sociální geografie</t>
   </si>
   <si>
@@ -688,42 +688,42 @@
     <t>Ap. biolog., ekolog. a ochrana biodiver.</t>
   </si>
   <si>
+    <t>Obecná fyzika a chemie</t>
+  </si>
+  <si>
     <t>Aplikovaná chemie</t>
   </si>
   <si>
-    <t>Obecná fyzika a chemie</t>
+    <t>Nanotechnologie a nanomateriály</t>
   </si>
   <si>
     <t>Syntéza, technologie a analýza</t>
   </si>
   <si>
-    <t>Nanotechnologie a nanomateriály</t>
-  </si>
-  <si>
     <t>Aplikovaná informatika: povinný základ</t>
   </si>
   <si>
     <t>Sociální geografie a územní rozvoj</t>
   </si>
   <si>
+    <t>Učitelství informatiky pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství geografie pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství biologie pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství fyziky pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství chemie pro střední školy</t>
+  </si>
+  <si>
     <t>Učitelství matematiky pro střední školy</t>
   </si>
   <si>
-    <t>Učitelství informatiky pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství chemie pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství biologie pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství fyziky pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství geografie pro střední školy</t>
-  </si>
-  <si>
     <t>Teoretické základy datového inženýrství</t>
   </si>
   <si>
@@ -772,12 +772,12 @@
     <t>Chemické inženýrství</t>
   </si>
   <si>
+    <t>Matematika s didaktikou</t>
+  </si>
+  <si>
     <t>Geografie s didaktikou pro ZŠ</t>
   </si>
   <si>
-    <t>Matematika s didaktikou</t>
-  </si>
-  <si>
     <t>Biologie s didaktikou</t>
   </si>
   <si>
@@ -790,27 +790,27 @@
     <t>Fyzika s didaktikou pro SŠ</t>
   </si>
   <si>
+    <t>Toxikologie a analýza škodlivin</t>
+  </si>
+  <si>
+    <t>Numerická matematika</t>
+  </si>
+  <si>
     <t>Regionální geografie a regionální rozvoj Česka</t>
   </si>
   <si>
-    <t>Toxikologie a analýza škodlivin</t>
-  </si>
-  <si>
-    <t>Numerická matematika</t>
-  </si>
-  <si>
     <t>Regionální geografie Evropy a světa</t>
   </si>
   <si>
     <t>Fyzická geografie</t>
   </si>
   <si>
+    <t>Informatika</t>
+  </si>
+  <si>
     <t>Geografie</t>
   </si>
   <si>
-    <t>Informatika</t>
-  </si>
-  <si>
     <t>Obecná geografie</t>
   </si>
   <si>
@@ -823,10 +823,10 @@
     <t>Aplikovaná biologie, ekologie a ochrana biodiverzity</t>
   </si>
   <si>
+    <t>Nanotechnologie a nanomateriály, jejich příprava a charakterizace</t>
+  </si>
+  <si>
     <t>Syntéza, technologie a analýza chemických látek a materiálů</t>
-  </si>
-  <si>
-    <t>Nanotechnologie a nanomateriály, jejich příprava a charakterizace</t>
   </si>
 </sst>
 </file>
@@ -1928,7 +1928,7 @@
         <v>145</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>145</v>
+        <v>249</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -1944,7 +1944,7 @@
         <v>146</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>249</v>
+        <v>146</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2565,10 +2565,10 @@
         <v>2023</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -2581,10 +2581,10 @@
         <v>2023</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -2600,7 +2600,7 @@
         <v>170</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -2744,7 +2744,7 @@
         <v>181</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>209</v>
+        <v>256</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -2760,7 +2760,7 @@
         <v>182</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -2776,7 +2776,7 @@
         <v>183</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>256</v>
+        <v>183</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -2824,7 +2824,7 @@
         <v>186</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>257</v>
+        <v>186</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
@@ -2856,7 +2856,7 @@
         <v>188</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>188</v>
+        <v>257</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
@@ -3048,7 +3048,7 @@
         <v>200</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
@@ -3064,7 +3064,7 @@
         <v>201</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -3077,10 +3077,10 @@
         <v>2023</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>261</v>
+        <v>200</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -3093,10 +3093,10 @@
         <v>2023</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>201</v>
+        <v>261</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -3173,10 +3173,10 @@
         <v>2023</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
@@ -3189,10 +3189,10 @@
         <v>2023</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -3237,10 +3237,10 @@
         <v>2023</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>173</v>
+        <v>264</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
@@ -3253,10 +3253,10 @@
         <v>2023</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>210</v>
+        <v>173</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>264</v>
+        <v>173</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -3272,7 +3272,7 @@
         <v>211</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>211</v>
+        <v>265</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -3304,7 +3304,7 @@
         <v>213</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>265</v>
+        <v>213</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
@@ -3381,10 +3381,10 @@
         <v>2023</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -3397,10 +3397,10 @@
         <v>2023</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -3413,10 +3413,10 @@
         <v>2023</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -3429,10 +3429,10 @@
         <v>2023</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
@@ -3509,10 +3509,10 @@
         <v>2023</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
@@ -3541,10 +3541,10 @@
         <v>2023</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>182</v>
+        <v>267</v>
       </c>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
@@ -3557,10 +3557,10 @@
         <v>2023</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>267</v>
+        <v>183</v>
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>

</xml_diff>

<commit_message>
Pohled fakulty: Join fix a generování učitelů
- Fakulta nyní znovugeneruje číselník učitelů
- Správné joinování předmětů se stejnými zkratkami ale jinými katedrami
</commit_message>
<xml_diff>
--- a/results/bez_garanta.xlsx
+++ b/results/bez_garanta.xlsx
@@ -433,12 +433,12 @@
     <t>Úvod do molekulárních simulací</t>
   </si>
   <si>
+    <t>Bakalářská práce z chemie</t>
+  </si>
+  <si>
     <t>Bakalářská práce z fyziky</t>
   </si>
   <si>
-    <t>Bakalářská práce z chemie</t>
-  </si>
-  <si>
     <t>PVK - Elektronika II</t>
   </si>
   <si>
@@ -451,12 +451,12 @@
     <t>PVK - Mikroprocesorová technika</t>
   </si>
   <si>
+    <t>Biochemická cvičení</t>
+  </si>
+  <si>
     <t>PVK - Automatizované měřící systémy</t>
   </si>
   <si>
-    <t>Biochemická cvičení</t>
-  </si>
-  <si>
     <t>Diplomová práce z chemie</t>
   </si>
   <si>
@@ -526,25 +526,28 @@
     <t>Anglický jazyk pro doktorandy</t>
   </si>
   <si>
+    <t>SZZ - biologie s didaktikou</t>
+  </si>
+  <si>
+    <t>SZZ - Geografie s didaktikou</t>
+  </si>
+  <si>
     <t>SZZ - matematika s didaktikou</t>
   </si>
   <si>
-    <t>SZZ - Geografie s didaktikou</t>
-  </si>
-  <si>
-    <t>SZZ - biologie s didaktikou</t>
-  </si>
-  <si>
     <t>Biologie</t>
   </si>
   <si>
+    <t>Aplikovaná fyzika</t>
+  </si>
+  <si>
+    <t>Aplikovaná geografie - Cestovní ruch</t>
+  </si>
+  <si>
     <t>Softwarové systémy</t>
   </si>
   <si>
-    <t>Aplikovaná fyzika</t>
-  </si>
-  <si>
-    <t>Aplikovaná geografie - Cestovní ruch</t>
+    <t>Informační technologie</t>
   </si>
   <si>
     <t>Nanotechnologie</t>
@@ -553,30 +556,27 @@
     <t>Aplikovaná geografie - Krajina a GIS</t>
   </si>
   <si>
-    <t>Informační technologie</t>
-  </si>
-  <si>
     <t>Matematika s aplikacemi</t>
   </si>
   <si>
+    <t>Počítačové modelování</t>
+  </si>
+  <si>
     <t>SZZ - Evropská integrace a EU</t>
   </si>
   <si>
     <t>SZZ - Chemie</t>
   </si>
   <si>
-    <t>Počítačové modelování</t>
-  </si>
-  <si>
     <t>Statistika a zpracování dat</t>
   </si>
   <si>
+    <t>Geografie krajiny a GIS</t>
+  </si>
+  <si>
     <t>Chemie a didaktika chemie pro SŠ</t>
   </si>
   <si>
-    <t>Geografie krajiny a GIS</t>
-  </si>
-  <si>
     <t>Biologie s didaktikou pro SŠ</t>
   </si>
   <si>
@@ -589,28 +589,31 @@
     <t>Regionální geografie a cestovní ruch</t>
   </si>
   <si>
+    <t>SZZ - Reg. geografie a reg. rozvoj Česka</t>
+  </si>
+  <si>
+    <t>SZZ - numerická matematika</t>
+  </si>
+  <si>
     <t>SZZ - Toxikologie a analýza škodlivin</t>
   </si>
   <si>
-    <t>SZZ - numerická matematika</t>
-  </si>
-  <si>
-    <t>SZZ - Reg. geografie a reg. rozvoj Česka</t>
+    <t>Geografie pro vzdělávání</t>
+  </si>
+  <si>
+    <t>Chemie pro vzdělávání</t>
   </si>
   <si>
     <t>Biologie pro vzdělávání</t>
   </si>
   <si>
-    <t>Geografie pro vzdělávání</t>
+    <t>Matematika pro vzdělávání</t>
   </si>
   <si>
     <t>Fyzika pro vzdělávání</t>
   </si>
   <si>
-    <t>Matematika pro vzdělávání</t>
-  </si>
-  <si>
-    <t>Chemie pro vzdělávání</t>
+    <t>SZZ - Biologie</t>
   </si>
   <si>
     <t>Analytická chemie</t>
@@ -619,9 +622,6 @@
     <t>Fyzika</t>
   </si>
   <si>
-    <t>SZZ - Biologie</t>
-  </si>
-  <si>
     <t>SZZ- Regionální geografie Evropy a světa</t>
   </si>
   <si>
@@ -640,24 +640,24 @@
     <t>Matematika</t>
   </si>
   <si>
+    <t>Chemie</t>
+  </si>
+  <si>
     <t>SZZ - Informatika</t>
   </si>
   <si>
-    <t>Chemie</t>
-  </si>
-  <si>
     <t>SZZ - Geografie</t>
   </si>
   <si>
     <t>SZZ - Obecná geografie</t>
   </si>
   <si>
+    <t>Elektronika a elektrotechnika</t>
+  </si>
+  <si>
     <t>Matematická informatika</t>
   </si>
   <si>
-    <t>Elektronika a elektrotechnika</t>
-  </si>
-  <si>
     <t>SZZ - Sociální geografie</t>
   </si>
   <si>
@@ -706,21 +706,21 @@
     <t>Sociální geografie a územní rozvoj</t>
   </si>
   <si>
+    <t>Učitelství geografie pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství fyziky pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství chemie pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství biologie pro střední školy</t>
+  </si>
+  <si>
     <t>Učitelství informatiky pro střední školy</t>
   </si>
   <si>
-    <t>Učitelství geografie pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství biologie pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství fyziky pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství chemie pro střední školy</t>
-  </si>
-  <si>
     <t>Učitelství matematiky pro střední školy</t>
   </si>
   <si>
@@ -772,15 +772,15 @@
     <t>Chemické inženýrství</t>
   </si>
   <si>
+    <t>Biologie s didaktikou</t>
+  </si>
+  <si>
+    <t>Geografie s didaktikou pro ZŠ</t>
+  </si>
+  <si>
     <t>Matematika s didaktikou</t>
   </si>
   <si>
-    <t>Geografie s didaktikou pro ZŠ</t>
-  </si>
-  <si>
-    <t>Biologie s didaktikou</t>
-  </si>
-  <si>
     <t>Geografie s didaktikou pro SŠ</t>
   </si>
   <si>
@@ -790,13 +790,13 @@
     <t>Fyzika s didaktikou pro SŠ</t>
   </si>
   <si>
+    <t>Regionální geografie a regionální rozvoj Česka</t>
+  </si>
+  <si>
+    <t>Numerická matematika</t>
+  </si>
+  <si>
     <t>Toxikologie a analýza škodlivin</t>
-  </si>
-  <si>
-    <t>Numerická matematika</t>
-  </si>
-  <si>
-    <t>Regionální geografie a regionální rozvoj Česka</t>
   </si>
   <si>
     <t>Regionální geografie Evropy a světa</t>
@@ -1928,7 +1928,7 @@
         <v>145</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>249</v>
+        <v>145</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -1944,7 +1944,7 @@
         <v>146</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>146</v>
+        <v>249</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2405,10 +2405,10 @@
         <v>2023</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -2421,10 +2421,10 @@
         <v>2023</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -2565,10 +2565,10 @@
         <v>2023</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -2597,10 +2597,10 @@
         <v>2023</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -2744,7 +2744,7 @@
         <v>181</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>256</v>
+        <v>181</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -2760,7 +2760,7 @@
         <v>182</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>209</v>
+        <v>256</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -2776,7 +2776,7 @@
         <v>183</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -3032,7 +3032,7 @@
         <v>199</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -3064,7 +3064,7 @@
         <v>201</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -3077,10 +3077,10 @@
         <v>2023</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -3173,10 +3173,10 @@
         <v>2023</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
@@ -3189,10 +3189,10 @@
         <v>2023</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -3208,7 +3208,7 @@
         <v>208</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>263</v>
+        <v>208</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -3224,7 +3224,7 @@
         <v>209</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>209</v>
+        <v>263</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -3381,10 +3381,10 @@
         <v>2023</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -3397,10 +3397,10 @@
         <v>2023</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -3413,10 +3413,10 @@
         <v>2023</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -3509,10 +3509,10 @@
         <v>2023</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
@@ -3525,10 +3525,10 @@
         <v>2023</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
@@ -3541,10 +3541,10 @@
         <v>2023</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>222</v>
+        <v>181</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>267</v>
+        <v>181</v>
       </c>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
@@ -3557,10 +3557,10 @@
         <v>2023</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>183</v>
+        <v>222</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>183</v>
+        <v>267</v>
       </c>
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>

</xml_diff>

<commit_message>
Malý úpravy v rámci čitelnosti
</commit_message>
<xml_diff>
--- a/results/bez_garanta.xlsx
+++ b/results/bez_garanta.xlsx
@@ -433,12 +433,12 @@
     <t>Úvod do molekulárních simulací</t>
   </si>
   <si>
+    <t>Bakalářská práce z fyziky</t>
+  </si>
+  <si>
     <t>Bakalářská práce z chemie</t>
   </si>
   <si>
-    <t>Bakalářská práce z fyziky</t>
-  </si>
-  <si>
     <t>PVK - Elektronika II</t>
   </si>
   <si>
@@ -526,33 +526,33 @@
     <t>Anglický jazyk pro doktorandy</t>
   </si>
   <si>
+    <t>SZZ - matematika s didaktikou</t>
+  </si>
+  <si>
     <t>SZZ - biologie s didaktikou</t>
   </si>
   <si>
     <t>SZZ - Geografie s didaktikou</t>
   </si>
   <si>
-    <t>SZZ - matematika s didaktikou</t>
-  </si>
-  <si>
     <t>Biologie</t>
   </si>
   <si>
     <t>Aplikovaná fyzika</t>
   </si>
   <si>
+    <t>Softwarové systémy</t>
+  </si>
+  <si>
     <t>Aplikovaná geografie - Cestovní ruch</t>
   </si>
   <si>
-    <t>Softwarové systémy</t>
+    <t>Nanotechnologie</t>
   </si>
   <si>
     <t>Informační technologie</t>
   </si>
   <si>
-    <t>Nanotechnologie</t>
-  </si>
-  <si>
     <t>Aplikovaná geografie - Krajina a GIS</t>
   </si>
   <si>
@@ -562,66 +562,66 @@
     <t>Počítačové modelování</t>
   </si>
   <si>
+    <t>SZZ - Chemie</t>
+  </si>
+  <si>
     <t>SZZ - Evropská integrace a EU</t>
   </si>
   <si>
-    <t>SZZ - Chemie</t>
-  </si>
-  <si>
     <t>Statistika a zpracování dat</t>
   </si>
   <si>
+    <t>SZZ - Fyzika s didaktikou pro SŠ</t>
+  </si>
+  <si>
     <t>Geografie krajiny a GIS</t>
   </si>
   <si>
+    <t>Biologie s didaktikou pro SŠ</t>
+  </si>
+  <si>
     <t>Chemie a didaktika chemie pro SŠ</t>
   </si>
   <si>
-    <t>Biologie s didaktikou pro SŠ</t>
-  </si>
-  <si>
-    <t>SZZ - Fyzika s didaktikou pro SŠ</t>
-  </si>
-  <si>
     <t>Geografie venkova a sídel</t>
   </si>
   <si>
     <t>Regionální geografie a cestovní ruch</t>
   </si>
   <si>
+    <t>SZZ - Toxikologie a analýza škodlivin</t>
+  </si>
+  <si>
+    <t>SZZ - numerická matematika</t>
+  </si>
+  <si>
     <t>SZZ - Reg. geografie a reg. rozvoj Česka</t>
   </si>
   <si>
-    <t>SZZ - numerická matematika</t>
-  </si>
-  <si>
-    <t>SZZ - Toxikologie a analýza škodlivin</t>
+    <t>Chemie pro vzdělávání</t>
+  </si>
+  <si>
+    <t>Fyzika pro vzdělávání</t>
+  </si>
+  <si>
+    <t>Matematika pro vzdělávání</t>
+  </si>
+  <si>
+    <t>Biologie pro vzdělávání</t>
   </si>
   <si>
     <t>Geografie pro vzdělávání</t>
   </si>
   <si>
-    <t>Chemie pro vzdělávání</t>
-  </si>
-  <si>
-    <t>Biologie pro vzdělávání</t>
-  </si>
-  <si>
-    <t>Matematika pro vzdělávání</t>
-  </si>
-  <si>
-    <t>Fyzika pro vzdělávání</t>
+    <t>Analytická chemie</t>
+  </si>
+  <si>
+    <t>Fyzika</t>
   </si>
   <si>
     <t>SZZ - Biologie</t>
   </si>
   <si>
-    <t>Analytická chemie</t>
-  </si>
-  <si>
-    <t>Fyzika</t>
-  </si>
-  <si>
     <t>SZZ- Regionální geografie Evropy a světa</t>
   </si>
   <si>
@@ -637,27 +637,27 @@
     <t>SZZ - Fyzická geografie</t>
   </si>
   <si>
+    <t>Chemie</t>
+  </si>
+  <si>
+    <t>SZZ - Informatika</t>
+  </si>
+  <si>
+    <t>SZZ - Geografie</t>
+  </si>
+  <si>
     <t>Matematika</t>
   </si>
   <si>
-    <t>Chemie</t>
-  </si>
-  <si>
-    <t>SZZ - Informatika</t>
-  </si>
-  <si>
-    <t>SZZ - Geografie</t>
+    <t>Elektronika a elektrotechnika</t>
+  </si>
+  <si>
+    <t>Matematická informatika</t>
   </si>
   <si>
     <t>SZZ - Obecná geografie</t>
   </si>
   <si>
-    <t>Elektronika a elektrotechnika</t>
-  </si>
-  <si>
-    <t>Matematická informatika</t>
-  </si>
-  <si>
     <t>SZZ - Sociální geografie</t>
   </si>
   <si>
@@ -688,36 +688,36 @@
     <t>Ap. biolog., ekolog. a ochrana biodiver.</t>
   </si>
   <si>
+    <t>Aplikovaná chemie</t>
+  </si>
+  <si>
     <t>Obecná fyzika a chemie</t>
   </si>
   <si>
-    <t>Aplikovaná chemie</t>
+    <t>Syntéza, technologie a analýza</t>
   </si>
   <si>
     <t>Nanotechnologie a nanomateriály</t>
   </si>
   <si>
-    <t>Syntéza, technologie a analýza</t>
-  </si>
-  <si>
     <t>Aplikovaná informatika: povinný základ</t>
   </si>
   <si>
     <t>Sociální geografie a územní rozvoj</t>
   </si>
   <si>
+    <t>Učitelství biologie pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství fyziky pro střední školy</t>
+  </si>
+  <si>
+    <t>Učitelství chemie pro střední školy</t>
+  </si>
+  <si>
     <t>Učitelství geografie pro střední školy</t>
   </si>
   <si>
-    <t>Učitelství fyziky pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství chemie pro střední školy</t>
-  </si>
-  <si>
-    <t>Učitelství biologie pro střední školy</t>
-  </si>
-  <si>
     <t>Učitelství informatiky pro střední školy</t>
   </si>
   <si>
@@ -772,15 +772,15 @@
     <t>Chemické inženýrství</t>
   </si>
   <si>
+    <t>Matematika s didaktikou</t>
+  </si>
+  <si>
     <t>Biologie s didaktikou</t>
   </si>
   <si>
     <t>Geografie s didaktikou pro ZŠ</t>
   </si>
   <si>
-    <t>Matematika s didaktikou</t>
-  </si>
-  <si>
     <t>Geografie s didaktikou pro SŠ</t>
   </si>
   <si>
@@ -790,15 +790,15 @@
     <t>Fyzika s didaktikou pro SŠ</t>
   </si>
   <si>
+    <t>Toxikologie a analýza škodlivin</t>
+  </si>
+  <si>
+    <t>Numerická matematika</t>
+  </si>
+  <si>
     <t>Regionální geografie a regionální rozvoj Česka</t>
   </si>
   <si>
-    <t>Numerická matematika</t>
-  </si>
-  <si>
-    <t>Toxikologie a analýza škodlivin</t>
-  </si>
-  <si>
     <t>Regionální geografie Evropy a světa</t>
   </si>
   <si>
@@ -823,10 +823,10 @@
     <t>Aplikovaná biologie, ekologie a ochrana biodiverzity</t>
   </si>
   <si>
+    <t>Syntéza, technologie a analýza chemických látek a materiálů</t>
+  </si>
+  <si>
     <t>Nanotechnologie a nanomateriály, jejich příprava a charakterizace</t>
-  </si>
-  <si>
-    <t>Syntéza, technologie a analýza chemických látek a materiálů</t>
   </si>
 </sst>
 </file>
@@ -2405,10 +2405,10 @@
         <v>2023</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -2421,10 +2421,10 @@
         <v>2023</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -2565,10 +2565,10 @@
         <v>2023</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -2581,10 +2581,10 @@
         <v>2023</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -2600,7 +2600,7 @@
         <v>171</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -2760,7 +2760,7 @@
         <v>182</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -2776,7 +2776,7 @@
         <v>183</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>208</v>
+        <v>256</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -2808,7 +2808,7 @@
         <v>185</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>185</v>
+        <v>257</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
@@ -2856,7 +2856,7 @@
         <v>188</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>257</v>
+        <v>188</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
@@ -3032,7 +3032,7 @@
         <v>199</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -3064,7 +3064,7 @@
         <v>201</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -3077,10 +3077,10 @@
         <v>2023</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>201</v>
+        <v>261</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -3093,10 +3093,10 @@
         <v>2023</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>261</v>
+        <v>200</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -3189,10 +3189,10 @@
         <v>2023</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -3208,7 +3208,7 @@
         <v>208</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>208</v>
+        <v>263</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -3224,7 +3224,7 @@
         <v>209</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -3240,7 +3240,7 @@
         <v>210</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>264</v>
+        <v>210</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
@@ -3272,7 +3272,7 @@
         <v>211</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>265</v>
+        <v>211</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -3304,7 +3304,7 @@
         <v>213</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>213</v>
+        <v>265</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
@@ -3381,10 +3381,10 @@
         <v>2023</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -3397,10 +3397,10 @@
         <v>2023</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -3509,10 +3509,10 @@
         <v>2023</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
@@ -3525,10 +3525,10 @@
         <v>2023</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>

</xml_diff>